<commit_message>
chore : code refactor
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://equancy-my.sharepoint.com/personal/sbouchenak_equancy_com/Documents/Bureau/Docs/calendar_app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Desktop\divers\training\calendar_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{ACBB5F33-B975-47AD-AE14-6BCB1E6AC81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28507FE0-9D9E-46EF-90F2-1B0C43D08816}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2850FA-75E6-44A9-9DC2-55694789A800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{0083B9F2-C954-45F5-9AC1-D8F8D2C39715}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0083B9F2-C954-45F5-9AC1-D8F8D2C39715}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Task</t>
   </si>
@@ -50,19 +39,28 @@
     <t>Frequency (days)</t>
   </si>
   <si>
-    <t>Meeting</t>
-  </si>
-  <si>
-    <t>Report Due</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Payroll</t>
-  </si>
-  <si>
     <t>Heure</t>
+  </si>
+  <si>
+    <t>HP VIC</t>
+  </si>
+  <si>
+    <t>Welcome Jouerney</t>
+  </si>
+  <si>
+    <t>Category Affinity</t>
+  </si>
+  <si>
+    <t>Product reco</t>
+  </si>
+  <si>
+    <t>One timer</t>
+  </si>
+  <si>
+    <t>Time to purchase</t>
+  </si>
+  <si>
+    <t>Product repurchase</t>
   </si>
 </sst>
 </file>
@@ -106,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -120,6 +118,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,13 +458,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2812D38A-18EF-416F-9E95-5AF1B6AE444E}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -482,67 +484,123 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>45717</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
       <c r="E2" s="4">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
-        <v>45721</v>
+        <v>45717</v>
       </c>
       <c r="C3" s="2">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="4">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
-        <v>45723</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
+        <v>45719</v>
+      </c>
+      <c r="C4" s="2">
         <v>7</v>
       </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="4">
-        <v>0.41666666666666669</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45717</v>
+      </c>
+      <c r="C5" s="2">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
-        <v>45726</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2">
+      <c r="D5" s="2"/>
+      <c r="E5" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>45717</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="B7" s="5">
+        <v>45717</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6">
         <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5">
+        <v>45719</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5">
+        <v>45722</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.70833333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : add pages to the app
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Desktop\divers\training\calendar_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://equancy-my.sharepoint.com/personal/sbouchenak_equancy_com/Documents/Bureau/Docs/calendar_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2850FA-75E6-44A9-9DC2-55694789A800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{DA2850FA-75E6-44A9-9DC2-55694789A800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FCB611A-3690-463C-9CAE-4D55D183A06C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0083B9F2-C954-45F5-9AC1-D8F8D2C39715}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0083B9F2-C954-45F5-9AC1-D8F8D2C39715}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -39,15 +39,9 @@
     <t>Frequency (days)</t>
   </si>
   <si>
-    <t>Heure</t>
-  </si>
-  <si>
     <t>HP VIC</t>
   </si>
   <si>
-    <t>Welcome Jouerney</t>
-  </si>
-  <si>
     <t>Category Affinity</t>
   </si>
   <si>
@@ -61,6 +55,27 @@
   </si>
   <si>
     <t>Product repurchase</t>
+  </si>
+  <si>
+    <t>Welcome Journey</t>
+  </si>
+  <si>
+    <t>GROUP</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>INGESTION</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>Segmentation</t>
+  </si>
+  <si>
+    <t>Hour</t>
   </si>
 </sst>
 </file>
@@ -119,7 +134,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,149 +473,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2812D38A-18EF-416F-9E95-5AF1B6AE444E}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="3">
+        <v>45717</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45717</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C4" s="3">
+        <v>45719</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45720</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5">
         <v>45717</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45717</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45719</v>
+      </c>
+      <c r="D8" s="2">
         <v>7</v>
       </c>
-      <c r="E2" s="4">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="F8" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45722</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="5">
         <v>45717</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>45719</v>
-      </c>
-      <c r="C4" s="2">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4">
-        <v>0.79166666666666663</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="F10" s="4">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5">
         <v>45717</v>
       </c>
-      <c r="C5" s="2">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4">
-        <v>0.29166666666666669</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5">
-        <v>45717</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5">
-        <v>45717</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="5">
-        <v>45719</v>
-      </c>
-      <c r="C8" s="2">
-        <v>7</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5">
-        <v>45722</v>
-      </c>
-      <c r="C9" s="2">
-        <v>7</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.70833333333333337</v>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.77083333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>